<commit_message>
[FIX] dunia perseederan product customer lead
</commit_message>
<xml_diff>
--- a/packages/sms-backend/public/products.xlsx
+++ b/packages/sms-backend/public/products.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>subscribtion_user_id</t>
   </si>
@@ -78,19 +78,79 @@
   </si>
   <si>
     <t>Asuransi Proyek</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/14/64ec4cfcac371_2023-tesla-model-x-101-1671475309.jpeg</t>
+  </si>
+  <si>
+    <t>https://img.freepik.com/premium-photo/crawler-buldozer-illustration-transportation-illustration-generative-ai_710947-95.jpg</t>
+  </si>
+  <si>
+    <t>https://chakrajawara.co.id/media/nwddpddh/mengenal-mesin-diesel-common-rail-tdi-dan-diesel-konvensional.png</t>
+  </si>
+  <si>
+    <t>Nissan GT-R</t>
+  </si>
+  <si>
+    <t>Mazda RX-7 VeilSide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSX 1000rr </t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/15/64ec4d60f0f7e_2021-nissan-gt-r-2457-3-1664901335.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/13/64ec4cb1f20df_IMG-20200506-WA0004-e1588733192512.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/30/64ed5c2e310a8_maxresdefault.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/8/64ec4a9200e31_5fdebc94f4196.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/12/64ec4bb7ee80c_32127_24959.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/7/64ec4a5a50cf3_lampukristal.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/11/64ec4b710dd2c_Screen-Shot-2023-08-28-at-14.23.16.png</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/10/64ec4b4b857b9_nationwide-mutual-insurance-company4591.jpeg</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/9/64ec4b031884a_insurance.jpeg</t>
+  </si>
+  <si>
+    <t>FWD Soul Insurance</t>
+  </si>
+  <si>
+    <t>https://melandas-production.s3.ap-southeast-1.amazonaws.com/21/64ec59cd9475f_HQT8RYW6SJSGMP2YJVJV-59523127.jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,8 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,7 +474,7 @@
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +502,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -470,8 +534,11 @@
       <c r="I2">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -499,8 +566,11 @@
       <c r="I3">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -528,179 +598,328 @@
       <c r="I4">
         <v>3000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10004</v>
+      </c>
+      <c r="H5">
+        <v>2000000</v>
+      </c>
+      <c r="I5">
+        <v>2000000</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>10005</v>
+      </c>
+      <c r="H6">
+        <v>3000000</v>
+      </c>
+      <c r="I6">
+        <v>3000000</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>10006</v>
+      </c>
+      <c r="H7">
+        <v>1800000</v>
+      </c>
+      <c r="I7">
+        <v>1800000</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="G5">
+      <c r="G8">
         <v>20001</v>
       </c>
-      <c r="H5">
+      <c r="H8">
         <v>100000000</v>
       </c>
-      <c r="I5">
+      <c r="I8">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="G6">
+      <c r="G9">
         <v>20002</v>
       </c>
-      <c r="H6">
+      <c r="H9">
         <v>20000000</v>
       </c>
-      <c r="I6">
+      <c r="I9">
         <v>20000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="G7">
+      <c r="G10">
         <v>20003</v>
       </c>
-      <c r="H7">
+      <c r="H10">
         <v>5000000</v>
       </c>
-      <c r="I7">
+      <c r="I10">
         <v>5000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="G11">
         <v>30001</v>
       </c>
-      <c r="H8">
+      <c r="H11">
         <v>1000000</v>
       </c>
-      <c r="I8">
+      <c r="I11">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="G9">
+      <c r="G12">
         <v>30002</v>
       </c>
-      <c r="H9">
+      <c r="H12">
         <v>2000000</v>
       </c>
-      <c r="I9">
+      <c r="I12">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="G10">
+      <c r="G13">
         <v>30003</v>
       </c>
-      <c r="H10">
+      <c r="H13">
         <v>3000000</v>
       </c>
-      <c r="I10">
+      <c r="I13">
         <v>3000000</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <v>30004</v>
+      </c>
+      <c r="H14" s="1">
+        <v>17000000</v>
+      </c>
+      <c r="I14" s="1">
+        <v>17000000</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>